<commit_message>
Funcionan con buena precisión, pero hay que mejorar los modelos bastante.
</commit_message>
<xml_diff>
--- a/ParametrosPyhtonDeepLearning.xlsx
+++ b/ParametrosPyhtonDeepLearning.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saguadog/Documents/TesisSergioAguado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630AF7C5-F80F-AB44-B853-955FD4A919AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE39374-DF88-4241-B7E5-FCB6AACEFD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{CADEC303-B83A-D047-87A0-BF26D46C0F75}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{CADEC303-B83A-D047-87A0-BF26D46C0F75}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN_Python" sheetId="1" r:id="rId1"/>
-    <sheet name="CNN_Matlab" sheetId="2" r:id="rId2"/>
+    <sheet name="LSTM_Python" sheetId="3" r:id="rId2"/>
+    <sheet name="CNN_Matlab" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="26">
   <si>
     <t>Capa</t>
   </si>
@@ -107,12 +108,21 @@
   <si>
     <t>Interación 10</t>
   </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>LSTM</t>
+  </si>
+  <si>
+    <t>Dense</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +150,11 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF9BA2B1"/>
+      <name val=".AppleSystemUIFontMonospaced"/>
     </font>
   </fonts>
   <fills count="8">
@@ -274,11 +289,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -306,6 +318,12 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -315,9 +333,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,15 +456,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>20053</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>20051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>218574</xdr:colOff>
+      <xdr:colOff>521369</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>40105</xdr:rowOff>
+      <xdr:rowOff>178213</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -477,8 +493,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="8642684"/>
-          <a:ext cx="2705100" cy="3048000"/>
+          <a:off x="20053" y="8462209"/>
+          <a:ext cx="2987842" cy="3366583"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -492,13 +508,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>26737</xdr:rowOff>
+      <xdr:rowOff>26736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>231274</xdr:colOff>
+      <xdr:colOff>320842</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>92242</xdr:rowOff>
+      <xdr:rowOff>193528</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -527,8 +543,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="13081000"/>
-          <a:ext cx="2717800" cy="3073400"/>
+          <a:off x="0" y="13080999"/>
+          <a:ext cx="2807368" cy="3174687"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -546,9 +562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>231274</xdr:colOff>
+      <xdr:colOff>340894</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>65505</xdr:rowOff>
+      <xdr:rowOff>189469</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -578,7 +594,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="17465842"/>
-          <a:ext cx="2717800" cy="3073400"/>
+          <a:ext cx="2827420" cy="3197364"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -596,9 +612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>303464</xdr:colOff>
+      <xdr:colOff>374316</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>98926</xdr:rowOff>
+      <xdr:rowOff>178306</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -628,7 +644,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="46790" y="22111368"/>
-          <a:ext cx="2743200" cy="3073400"/>
+          <a:ext cx="2814052" cy="3152780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -646,9 +662,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>256674</xdr:colOff>
+      <xdr:colOff>347578</xdr:colOff>
       <xdr:row>138</xdr:row>
-      <xdr:rowOff>79543</xdr:rowOff>
+      <xdr:rowOff>180969</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -678,7 +694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="26716790"/>
-          <a:ext cx="2743200" cy="3060700"/>
+          <a:ext cx="2834104" cy="3162126"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -696,9 +712,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>304131</xdr:colOff>
+      <xdr:colOff>387685</xdr:colOff>
       <xdr:row>161</xdr:row>
-      <xdr:rowOff>92910</xdr:rowOff>
+      <xdr:rowOff>186568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -728,7 +744,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="60157" y="31342263"/>
-          <a:ext cx="2730500" cy="3060700"/>
+          <a:ext cx="2814054" cy="3154358"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -740,15 +756,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>33422</xdr:colOff>
+      <xdr:colOff>33421</xdr:colOff>
       <xdr:row>167</xdr:row>
       <xdr:rowOff>20052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>290096</xdr:colOff>
+      <xdr:colOff>327526</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>136358</xdr:rowOff>
+      <xdr:rowOff>178988</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -777,8 +793,113 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33422" y="35533263"/>
-          <a:ext cx="2743200" cy="3124200"/>
+          <a:off x="33421" y="35533263"/>
+          <a:ext cx="2780631" cy="3166830"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6683</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>6683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>354262</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>187156</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagen 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4470BADE-8A64-1353-3AC9-8A92EEB932EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6683" y="39730946"/>
+          <a:ext cx="2834105" cy="3188368"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>668397</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>155989</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE8C83D7-B19E-C5B2-E3BC-07F27F5B25D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1021522"/>
+          <a:ext cx="3153180" cy="3551858"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -791,21 +912,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>188</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>6902</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>256674</xdr:colOff>
-      <xdr:row>203</xdr:row>
-      <xdr:rowOff>78205</xdr:rowOff>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>151977</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Imagen 20">
+        <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4470BADE-8A64-1353-3AC9-8A92EEB932EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B545A8FC-A3AA-C0E2-8917-8B29C2C414BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -814,7 +935,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -827,8 +948,213 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="39724263"/>
-          <a:ext cx="2743200" cy="3086100"/>
+          <a:off x="0" y="5611467"/>
+          <a:ext cx="3119783" cy="3547846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>634297</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>6902</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>428095</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>144946</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A4DE655-BB0E-6C71-6B0D-55BD4D3CCE20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3119080" y="5625272"/>
+          <a:ext cx="2278580" cy="3540815"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>200162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>652054</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>103531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92D64A09-5FC8-9BA8-140A-76D602CD553A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10422282"/>
+          <a:ext cx="3136837" cy="3506303"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>651770</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>6901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>490055</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>109325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C180B3E8-66FB-3878-6B44-4CAC65BA0ABB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3136553" y="10429184"/>
+          <a:ext cx="2323067" cy="3505195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>46302</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>372533</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D3E115-9A23-E391-D01E-1C658D47103D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="46302" y="1455209"/>
+          <a:ext cx="2806700" cy="1435100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1159,1033 +1485,1033 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A27538-E3B8-AD45-A3E5-D9CDC9B54440}">
   <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140:F146"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E182" sqref="E182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="5" width="10.83203125" style="3"/>
+    <col min="2" max="5" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2">
+    <row r="2" spans="1:6">
+      <c r="A2" s="11"/>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>64</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5">
+    <row r="3" spans="1:6">
+      <c r="A3" s="11"/>
+      <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>32</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2">
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="11"/>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>32</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="11"/>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="175" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="175" customHeight="1"/>
+    <row r="7" spans="1:6">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2">
+    <row r="8" spans="1:6">
+      <c r="A8" s="11"/>
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>64</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="5">
+    <row r="9" spans="1:6">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>32</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2">
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="11"/>
+      <c r="B10" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="5">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="11"/>
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4">
         <v>7</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="F11" s="11"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2">
+    <row r="29" spans="1:6">
+      <c r="A29" s="11"/>
+      <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>64</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="E29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="5">
+    <row r="30" spans="1:6">
+      <c r="A30" s="11"/>
+      <c r="B30" s="4">
         <v>2</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>64</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2">
+      <c r="D30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="11"/>
+      <c r="B31" s="1">
         <v>3</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>32</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="5">
-        <v>4</v>
-      </c>
-      <c r="C32" s="5">
+      <c r="D31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="11"/>
+      <c r="B32" s="4">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4">
         <v>7</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="D32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="F32" s="11"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2">
+    <row r="51" spans="1:6">
+      <c r="A51" s="11"/>
+      <c r="B51" s="1">
         <v>1</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>64</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" s="1">
+      <c r="E51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-      <c r="B52" s="5">
+    <row r="52" spans="1:6">
+      <c r="A52" s="11"/>
+      <c r="B52" s="4">
         <v>2</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="4">
         <v>64</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2">
+      <c r="D52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="11"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="11"/>
+      <c r="B53" s="1">
         <v>3</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>32</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-      <c r="B54" s="5">
-        <v>4</v>
-      </c>
-      <c r="C54" s="5">
+      <c r="D53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="11"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="11"/>
+      <c r="B54" s="4">
+        <v>4</v>
+      </c>
+      <c r="C54" s="4">
         <v>32</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2">
+      <c r="D54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="11"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="11"/>
+      <c r="B55" s="1">
         <v>5</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>7</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" s="6" t="s">
+      <c r="D55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+      <c r="F55" s="11"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F72" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2">
+    <row r="73" spans="1:6">
+      <c r="A73" s="11"/>
+      <c r="B73" s="1">
         <v>1</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="1">
         <v>128</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F73" s="1">
+      <c r="E73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-      <c r="B74" s="5">
+    <row r="74" spans="1:6">
+      <c r="A74" s="11"/>
+      <c r="B74" s="4">
         <v>2</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="4">
         <v>64</v>
       </c>
-      <c r="D74" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-      <c r="B75" s="2">
+      <c r="D74" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="11"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="11"/>
+      <c r="B75" s="1">
         <v>3</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="1">
         <v>64</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-      <c r="B76" s="5">
-        <v>4</v>
-      </c>
-      <c r="C76" s="5">
+      <c r="D75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="11"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="11"/>
+      <c r="B76" s="4">
+        <v>4</v>
+      </c>
+      <c r="C76" s="4">
         <v>32</v>
       </c>
-      <c r="D76" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
-      <c r="B77" s="2">
+      <c r="D76" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" s="11"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="11"/>
+      <c r="B77" s="1">
         <v>5</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="1">
         <v>7</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E77" s="6" t="s">
+      <c r="D77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+      <c r="F77" s="11"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E94" s="4" t="s">
+      <c r="E94" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F94" s="4" t="s">
+      <c r="F94" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="1"/>
-      <c r="B95" s="2">
+    <row r="95" spans="1:6">
+      <c r="A95" s="11"/>
+      <c r="B95" s="1">
         <v>1</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95" s="1">
         <v>128</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D95" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F95" s="1">
+      <c r="E95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F95" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="1"/>
-      <c r="B96" s="5">
+    <row r="96" spans="1:6">
+      <c r="A96" s="11"/>
+      <c r="B96" s="4">
         <v>2</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C96" s="4">
         <v>64</v>
       </c>
-      <c r="D96" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="1"/>
-      <c r="B97" s="2">
+      <c r="D96" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F96" s="11"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="11"/>
+      <c r="B97" s="1">
         <v>3</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97" s="1">
         <v>64</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="1"/>
-      <c r="B98" s="5">
-        <v>4</v>
-      </c>
-      <c r="C98" s="5">
+      <c r="D97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F97" s="11"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="11"/>
+      <c r="B98" s="4">
+        <v>4</v>
+      </c>
+      <c r="C98" s="4">
         <v>64</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="1"/>
-      <c r="B99" s="2">
+      <c r="D98" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F98" s="11"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="11"/>
+      <c r="B99" s="1">
         <v>5</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99" s="1">
         <v>32</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F99" s="1"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="1"/>
-      <c r="B100" s="5">
-        <v>6</v>
-      </c>
-      <c r="C100" s="5">
+      <c r="D99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F99" s="11"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="11"/>
+      <c r="B100" s="4">
+        <v>6</v>
+      </c>
+      <c r="C100" s="4">
         <v>7</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E100" s="5" t="s">
+      <c r="D100" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F100" s="1"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+      <c r="F100" s="11"/>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C117" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E117" s="4" t="s">
+      <c r="E117" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F117" s="4" t="s">
+      <c r="F117" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="1"/>
-      <c r="B118" s="2">
+    <row r="118" spans="1:6">
+      <c r="A118" s="11"/>
+      <c r="B118" s="1">
         <v>1</v>
       </c>
-      <c r="C118" s="2">
+      <c r="C118" s="1">
         <v>128</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="D118" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F118" s="1">
+      <c r="E118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F118" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="1"/>
-      <c r="B119" s="5">
+    <row r="119" spans="1:6">
+      <c r="A119" s="11"/>
+      <c r="B119" s="4">
         <v>2</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C119" s="4">
         <v>128</v>
       </c>
-      <c r="D119" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E119" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" s="1"/>
-      <c r="B120" s="2">
+      <c r="D119" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F119" s="11"/>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="11"/>
+      <c r="B120" s="1">
         <v>3</v>
       </c>
-      <c r="C120" s="2">
+      <c r="C120" s="1">
         <v>64</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F120" s="1"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="1"/>
-      <c r="B121" s="5">
-        <v>4</v>
-      </c>
-      <c r="C121" s="5">
+      <c r="D120" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F120" s="11"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="11"/>
+      <c r="B121" s="4">
+        <v>4</v>
+      </c>
+      <c r="C121" s="4">
         <v>64</v>
       </c>
-      <c r="D121" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="1"/>
-      <c r="B122" s="2">
+      <c r="D121" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F121" s="11"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="11"/>
+      <c r="B122" s="1">
         <v>5</v>
       </c>
-      <c r="C122" s="2">
+      <c r="C122" s="1">
         <v>32</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E122" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="1"/>
-      <c r="B123" s="5">
-        <v>6</v>
-      </c>
-      <c r="C123" s="5">
+      <c r="D122" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F122" s="11"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="11"/>
+      <c r="B123" s="4">
+        <v>6</v>
+      </c>
+      <c r="C123" s="4">
         <v>7</v>
       </c>
-      <c r="D123" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E123" s="5" t="s">
+      <c r="D123" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E123" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F123" s="1"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
+      <c r="F123" s="11"/>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C140" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D140" s="4" t="s">
+      <c r="D140" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E140" s="4" t="s">
+      <c r="E140" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F140" s="4" t="s">
+      <c r="F140" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A141" s="1"/>
-      <c r="B141" s="2">
+    <row r="141" spans="1:6">
+      <c r="A141" s="11"/>
+      <c r="B141" s="1">
         <v>1</v>
       </c>
-      <c r="C141" s="2">
+      <c r="C141" s="1">
         <v>256</v>
       </c>
-      <c r="D141" s="2" t="s">
+      <c r="D141" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E141" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F141" s="1">
+      <c r="E141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F141" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="1"/>
-      <c r="B142" s="5">
+    <row r="142" spans="1:6">
+      <c r="A142" s="11"/>
+      <c r="B142" s="4">
         <v>2</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C142" s="4">
         <v>128</v>
       </c>
-      <c r="D142" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E142" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F142" s="1"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143" s="1"/>
-      <c r="B143" s="2">
+      <c r="D142" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F142" s="11"/>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="11"/>
+      <c r="B143" s="1">
         <v>3</v>
       </c>
-      <c r="C143" s="2">
+      <c r="C143" s="1">
         <v>128</v>
       </c>
-      <c r="D143" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F143" s="1"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="1"/>
-      <c r="B144" s="5">
-        <v>4</v>
-      </c>
-      <c r="C144" s="5">
+      <c r="D143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F143" s="11"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="11"/>
+      <c r="B144" s="4">
+        <v>4</v>
+      </c>
+      <c r="C144" s="4">
         <v>64</v>
       </c>
-      <c r="D144" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E144" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F144" s="1"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="1"/>
-      <c r="B145" s="2">
+      <c r="D144" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F144" s="11"/>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="11"/>
+      <c r="B145" s="1">
         <v>5</v>
       </c>
-      <c r="C145" s="2">
+      <c r="C145" s="1">
         <v>32</v>
       </c>
-      <c r="D145" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E145" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F145" s="1"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" s="1"/>
-      <c r="B146" s="5">
-        <v>6</v>
-      </c>
-      <c r="C146" s="5">
+      <c r="D145" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F145" s="11"/>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="11"/>
+      <c r="B146" s="4">
+        <v>6</v>
+      </c>
+      <c r="C146" s="4">
         <v>7</v>
       </c>
-      <c r="D146" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E146" s="5" t="s">
+      <c r="D146" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E146" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F146" s="1"/>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A163" s="1" t="s">
+      <c r="F146" s="11"/>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B163" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C163" s="4" t="s">
+      <c r="C163" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D163" s="4" t="s">
+      <c r="D163" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E163" s="4" t="s">
+      <c r="E163" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F163" s="4" t="s">
+      <c r="F163" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G163" s="4" t="s">
+      <c r="G163" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A164" s="1"/>
-      <c r="B164" s="2">
+    <row r="164" spans="1:7">
+      <c r="A164" s="11"/>
+      <c r="B164" s="1">
         <v>1</v>
       </c>
-      <c r="C164" s="2">
+      <c r="C164" s="1">
         <v>256</v>
       </c>
-      <c r="D164" s="2" t="s">
+      <c r="D164" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E164" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F164" s="14">
+      <c r="E164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F164" s="10">
         <v>0</v>
       </c>
-      <c r="G164" s="1">
+      <c r="G164" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A165" s="1"/>
-      <c r="B165" s="5">
+    <row r="165" spans="1:7">
+      <c r="A165" s="11"/>
+      <c r="B165" s="4">
         <v>2</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C165" s="4">
         <v>128</v>
       </c>
-      <c r="D165" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E165" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F165" s="5" t="s">
+      <c r="D165" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F165" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G165" s="1"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A166" s="1"/>
-      <c r="B166" s="2">
+      <c r="G165" s="11"/>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" s="11"/>
+      <c r="B166" s="1">
         <v>3</v>
       </c>
-      <c r="C166" s="2">
+      <c r="C166" s="1">
         <v>32</v>
       </c>
-      <c r="D166" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F166" s="2" t="s">
+      <c r="D166" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F166" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G166" s="1"/>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A167" s="1"/>
-      <c r="B167" s="5">
-        <v>4</v>
-      </c>
-      <c r="C167" s="5">
+      <c r="G166" s="11"/>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" s="11"/>
+      <c r="B167" s="4">
+        <v>4</v>
+      </c>
+      <c r="C167" s="4">
         <v>7</v>
       </c>
-      <c r="D167" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E167" s="5" t="s">
+      <c r="D167" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E167" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F167" s="5">
+      <c r="F167" s="4">
         <v>0</v>
       </c>
-      <c r="G167" s="1"/>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A184" s="1" t="s">
+      <c r="G167" s="11"/>
+    </row>
+    <row r="184" spans="1:7">
+      <c r="A184" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C184" s="4" t="s">
+      <c r="C184" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D184" s="4" t="s">
+      <c r="D184" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E184" s="4" t="s">
+      <c r="E184" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F184" s="4" t="s">
+      <c r="F184" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G184" s="4" t="s">
+      <c r="G184" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A185" s="1"/>
-      <c r="B185" s="2">
+    <row r="185" spans="1:7">
+      <c r="A185" s="11"/>
+      <c r="B185" s="1">
         <v>1</v>
       </c>
-      <c r="C185" s="2">
+      <c r="C185" s="1">
         <v>128</v>
       </c>
-      <c r="D185" s="2" t="s">
+      <c r="D185" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E185" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F185" s="14">
+      <c r="E185" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F185" s="10">
         <v>0</v>
       </c>
-      <c r="G185" s="1">
+      <c r="G185" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A186" s="1"/>
-      <c r="B186" s="5">
+    <row r="186" spans="1:7">
+      <c r="A186" s="11"/>
+      <c r="B186" s="4">
         <v>2</v>
       </c>
-      <c r="C186" s="5">
+      <c r="C186" s="4">
         <v>64</v>
       </c>
-      <c r="D186" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E186" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F186" s="5" t="s">
+      <c r="D186" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E186" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F186" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G186" s="1"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A187" s="1"/>
-      <c r="B187" s="2">
+      <c r="G186" s="11"/>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" s="11"/>
+      <c r="B187" s="1">
         <v>3</v>
       </c>
-      <c r="C187" s="2">
+      <c r="C187" s="1">
         <v>32</v>
       </c>
-      <c r="D187" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E187" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F187" s="2" t="s">
+      <c r="D187" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F187" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G187" s="1"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A188" s="1"/>
-      <c r="B188" s="5">
-        <v>4</v>
-      </c>
-      <c r="C188" s="5">
+      <c r="G187" s="11"/>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" s="11"/>
+      <c r="B188" s="4">
+        <v>4</v>
+      </c>
+      <c r="C188" s="4">
         <v>7</v>
       </c>
-      <c r="D188" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E188" s="5" t="s">
+      <c r="D188" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E188" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F188" s="5">
+      <c r="F188" s="4">
         <v>0</v>
       </c>
-      <c r="G188" s="1"/>
+      <c r="G188" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -2216,132 +2542,479 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8716B53C-DBBA-604C-A42D-E8642A698BC2}">
+  <dimension ref="A1:G52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="11"/>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>128</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="11"/>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>64</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="11"/>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="11"/>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="17">
+      <c r="G16" s="15"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="11"/>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>128</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="11"/>
+      <c r="B26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4">
+        <v>64</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="11"/>
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
+        <v>32</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="11"/>
+      <c r="B28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="4">
+        <v>4</v>
+      </c>
+      <c r="D28" s="4">
+        <v>7</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="11"/>
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>128</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="11"/>
+      <c r="B49" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="4">
+        <v>2</v>
+      </c>
+      <c r="D49" s="4">
+        <v>64</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="11"/>
+      <c r="B50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>32</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="11"/>
+      <c r="B51" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="4">
+        <v>4</v>
+      </c>
+      <c r="D51" s="4">
+        <v>32</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="11"/>
+      <c r="B52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="1">
+        <v>5</v>
+      </c>
+      <c r="D52" s="1">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="G48:G52"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3201F3F4-F4AB-D345-BB53-655234BD09BD}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8">
+    <row r="2" spans="1:6">
+      <c r="A2" s="13"/>
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>256</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="11">
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="12">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="9">
+    <row r="3" spans="1:6">
+      <c r="A3" s="13"/>
+      <c r="B3" s="8">
         <v>2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>128</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="8">
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="13"/>
+      <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>128</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="9">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="13"/>
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
         <v>64</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="8">
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="13"/>
+      <c r="B6" s="7">
         <v>5</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>32</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="9">
-        <v>6</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="D6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14"/>
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
         <v>7</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2349,5 +3022,6 @@
     <mergeCell ref="F2:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>